<commit_message>
no permitir un trabajo con subwork y fip,ftp iguales
</commit_message>
<xml_diff>
--- a/public/reporteRudel2.xlsx
+++ b/public/reporteRudel2.xlsx
@@ -49,7 +49,7 @@
     <t>Ubicación del equipo:</t>
   </si>
   <si>
-    <t>Economizador II piso 6°, Buzón Eco 2</t>
+    <t>Economizador II piso 6°, Buzón Eco 6</t>
   </si>
   <si>
     <t>Supervisor turno día:</t>
@@ -91,7 +91,7 @@
     <t>Inicio</t>
   </si>
   <si>
-    <t>08/05/2017</t>
+    <t>25/05/2017</t>
   </si>
   <si>
     <t>Hora Inicio:</t>

</xml_diff>